<commit_message>
Subiendo proyecto completo de automatizacion de la pagina adida
</commit_message>
<xml_diff>
--- a/DatosRetoPom.xlsx
+++ b/DatosRetoPom.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18855" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="18855" windowHeight="8460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="url" sheetId="1" r:id="rId1"/>
     <sheet name="datoslogin" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="producto a buscar" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>URL</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>3145918290g</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>pantalones</t>
   </si>
 </sst>
 </file>
@@ -103,13 +109,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -439,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -476,12 +483,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>